<commit_message>
final touches on round scrapping
</commit_message>
<xml_diff>
--- a/webscrapping/matches/model/Book1.xlsx
+++ b/webscrapping/matches/model/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Meus Documentos\Python\Notebooks\Datascience\Classification_datascience\webscrapping\matches\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB0E5341-3E17-4D5C-8A8D-3F40F0E68B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26DC98F3-11BA-46D0-8505-2DCE4B536D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{1C43445C-3BFE-43FA-8FCA-AB69F1532CAF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{1C43445C-3BFE-43FA-8FCA-AB69F1532CAF}"/>
   </bookViews>
   <sheets>
     <sheet name="overview" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="economies" sheetId="3" r:id="rId3"/>
     <sheet name="events" sheetId="4" r:id="rId4"/>
     <sheet name="final_sheet" sheetId="5" r:id="rId5"/>
+    <sheet name="test" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="111">
   <si>
     <t>number</t>
   </si>
@@ -600,15 +601,9 @@
     <t>price</t>
   </si>
   <si>
-    <t>ATK_gun_price</t>
-  </si>
-  <si>
     <t>playerName</t>
   </si>
   <si>
-    <t>DEF_gun_price</t>
-  </si>
-  <si>
     <t>ATK_alive</t>
   </si>
   <si>
@@ -663,7 +658,25 @@
     <t>round_result</t>
   </si>
   <si>
-    <t>event id</t>
+    <t>avg_ATK_gun_price</t>
+  </si>
+  <si>
+    <t>avg_DEF_gun_price</t>
+  </si>
+  <si>
+    <t>matchId</t>
+  </si>
+  <si>
+    <t>eventId</t>
+  </si>
+  <si>
+    <t>best_of</t>
+  </si>
+  <si>
+    <t>mapId</t>
+  </si>
+  <si>
+    <t>'Icebox'</t>
   </si>
 </sst>
 </file>
@@ -3830,7 +3843,7 @@
   <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3861,13 +3874,13 @@
         <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>39</v>
@@ -4823,27 +4836,30 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F1A27BA-379F-49F7-9EA2-31A14ABA745C}">
-  <dimension ref="A1:T41"/>
+  <dimension ref="A1:X41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S1" sqref="A1:S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" customWidth="1"/>
     <col min="11" max="11" width="16.42578125" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.42578125" customWidth="1"/>
+    <col min="20" max="20" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4851,37 +4867,37 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>106</v>
+        <v>38</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>99</v>
@@ -4896,16 +4912,22 @@
         <v>102</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
+    </row>
+    <row r="2" spans="1:24">
       <c r="A2" s="1">
         <v>4</v>
       </c>
@@ -4913,25 +4935,25 @@
         <v>401753</v>
       </c>
       <c r="C2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="1">
-        <v>0</v>
+        <v>2900</v>
       </c>
       <c r="E2" s="1">
-        <v>14500</v>
+        <v>3320</v>
       </c>
       <c r="F2" s="1">
-        <v>16600</v>
+        <v>5</v>
       </c>
       <c r="G2" s="1">
         <v>5</v>
       </c>
       <c r="H2" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" s="1">
         <v>0</v>
@@ -4946,28 +4968,34 @@
         <v>0</v>
       </c>
       <c r="N2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O2" s="1">
         <v>0</v>
       </c>
       <c r="P2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q2" s="1">
         <v>0</v>
       </c>
       <c r="R2" s="1">
-        <v>0</v>
+        <v>12728</v>
       </c>
       <c r="S2" s="1">
-        <v>0</v>
-      </c>
-      <c r="T2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20">
+        <v>502</v>
+      </c>
+      <c r="V2" s="1">
+        <v>3</v>
+      </c>
+      <c r="W2" s="1">
+        <v>4</v>
+      </c>
+      <c r="X2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
       <c r="A3" s="1">
         <v>4</v>
       </c>
@@ -4975,26 +5003,25 @@
         <v>401753</v>
       </c>
       <c r="C3" s="1">
-        <v>2</v>
+        <v>7970</v>
       </c>
       <c r="D3" s="1">
-        <v>7970</v>
+        <v>2900</v>
       </c>
       <c r="E3" s="1">
-        <v>14500</v>
+        <v>2740</v>
       </c>
       <c r="F3" s="1">
-        <f>16600-2900</f>
-        <v>13700</v>
+        <v>5</v>
       </c>
       <c r="G3" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H3" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" s="1">
         <v>0</v>
@@ -5009,28 +5036,34 @@
         <v>0</v>
       </c>
       <c r="N3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3" s="1">
         <v>0</v>
       </c>
       <c r="P3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q3" s="1">
         <v>0</v>
       </c>
       <c r="R3" s="1">
-        <v>0</v>
+        <v>12728</v>
       </c>
       <c r="S3" s="1">
-        <v>0</v>
-      </c>
-      <c r="T3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
+        <v>502</v>
+      </c>
+      <c r="V3" s="1">
+        <v>3</v>
+      </c>
+      <c r="W3" s="1">
+        <v>4</v>
+      </c>
+      <c r="X3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -5038,32 +5071,31 @@
         <v>401753</v>
       </c>
       <c r="C4" s="1">
-        <v>3</v>
+        <v>22203</v>
       </c>
       <c r="D4" s="1">
-        <v>22203</v>
+        <v>2900</v>
       </c>
       <c r="E4" s="1">
-        <v>14500</v>
+        <v>2740</v>
       </c>
       <c r="F4" s="1">
-        <f>16600-2900</f>
-        <v>13700</v>
+        <v>5</v>
       </c>
       <c r="G4" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H4" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" s="1">
-        <v>0</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>98</v>
+        <v>1</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
       </c>
       <c r="L4" s="1">
         <v>0</v>
@@ -5072,28 +5104,34 @@
         <v>0</v>
       </c>
       <c r="N4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4" s="1">
         <v>0</v>
       </c>
       <c r="P4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="1">
         <v>0</v>
       </c>
       <c r="R4" s="1">
-        <v>0</v>
+        <v>12728</v>
       </c>
       <c r="S4" s="1">
-        <v>0</v>
-      </c>
-      <c r="T4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20">
+        <v>502</v>
+      </c>
+      <c r="V4" s="1">
+        <v>3</v>
+      </c>
+      <c r="W4" s="1">
+        <v>4</v>
+      </c>
+      <c r="X4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -5101,32 +5139,31 @@
         <v>401753</v>
       </c>
       <c r="C5" s="1">
-        <v>4</v>
+        <v>29211</v>
       </c>
       <c r="D5" s="1">
-        <v>29211</v>
+        <v>2320</v>
       </c>
       <c r="E5" s="1">
-        <v>11600</v>
+        <v>2740</v>
       </c>
       <c r="F5" s="1">
-        <v>13700</v>
+        <v>4</v>
       </c>
       <c r="G5" s="1">
         <v>4</v>
       </c>
       <c r="H5" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" s="1">
-        <f>D5-$D4</f>
-        <v>7008</v>
+        <v>0</v>
       </c>
       <c r="L5" s="1">
         <v>0</v>
@@ -5135,28 +5172,34 @@
         <v>0</v>
       </c>
       <c r="N5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5" s="1">
         <v>0</v>
       </c>
       <c r="P5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="1">
         <v>0</v>
       </c>
       <c r="R5" s="1">
-        <v>0</v>
+        <v>12728</v>
       </c>
       <c r="S5" s="1">
-        <v>0</v>
-      </c>
-      <c r="T5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20">
+        <v>502</v>
+      </c>
+      <c r="V5" s="1">
+        <v>3</v>
+      </c>
+      <c r="W5" s="1">
+        <v>4</v>
+      </c>
+      <c r="X5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -5164,62 +5207,67 @@
         <v>401753</v>
       </c>
       <c r="C6" s="1">
-        <v>5</v>
+        <v>50165</v>
       </c>
       <c r="D6" s="1">
-        <v>50165</v>
+        <v>2320</v>
       </c>
       <c r="E6" s="1">
-        <v>11600</v>
+        <v>2160</v>
       </c>
       <c r="F6" s="1">
-        <v>10800</v>
+        <v>4</v>
       </c>
       <c r="G6" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H6" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" s="1">
         <v>0</v>
       </c>
       <c r="K6" s="1">
-        <f>D6-$D4</f>
-        <v>27962</v>
+        <v>1</v>
       </c>
       <c r="L6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6" s="1">
         <v>0</v>
       </c>
       <c r="N6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6" s="1">
         <v>0</v>
       </c>
       <c r="P6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="1">
         <v>0</v>
       </c>
       <c r="R6" s="1">
-        <v>0</v>
+        <v>12728</v>
       </c>
       <c r="S6" s="1">
-        <v>0</v>
-      </c>
-      <c r="T6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20">
+        <v>502</v>
+      </c>
+      <c r="V6" s="1">
+        <v>3</v>
+      </c>
+      <c r="W6" s="1">
+        <v>4</v>
+      </c>
+      <c r="X6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -5227,62 +5275,67 @@
         <v>401753</v>
       </c>
       <c r="C7" s="1">
-        <v>6</v>
+        <v>50765</v>
       </c>
       <c r="D7" s="1">
-        <v>50765</v>
+        <v>1740</v>
       </c>
       <c r="E7" s="1">
-        <v>8700</v>
+        <v>2160</v>
       </c>
       <c r="F7" s="1">
-        <v>10800</v>
+        <v>3</v>
       </c>
       <c r="G7" s="1">
         <v>3</v>
       </c>
       <c r="H7" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="1">
         <v>0</v>
       </c>
       <c r="K7" s="1">
-        <f>D7-$D4</f>
-        <v>28562</v>
+        <v>1</v>
       </c>
       <c r="L7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7" s="1">
         <v>0</v>
       </c>
       <c r="N7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7" s="1">
         <v>0</v>
       </c>
       <c r="P7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q7" s="1">
         <v>0</v>
       </c>
       <c r="R7" s="1">
-        <v>0</v>
+        <v>12728</v>
       </c>
       <c r="S7" s="1">
-        <v>0</v>
-      </c>
-      <c r="T7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20">
+        <v>502</v>
+      </c>
+      <c r="V7" s="1">
+        <v>3</v>
+      </c>
+      <c r="W7" s="1">
+        <v>4</v>
+      </c>
+      <c r="X7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -5290,22 +5343,22 @@
         <v>401753</v>
       </c>
       <c r="C8" s="1">
-        <v>7</v>
+        <v>51696</v>
       </c>
       <c r="D8" s="1">
-        <v>51696</v>
+        <v>1740</v>
       </c>
       <c r="E8" s="1">
-        <v>8700</v>
+        <v>1160</v>
       </c>
       <c r="F8" s="1">
-        <v>5800</v>
+        <v>3</v>
       </c>
       <c r="G8" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H8" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I8" s="1">
         <v>0</v>
@@ -5314,38 +5367,43 @@
         <v>0</v>
       </c>
       <c r="K8" s="1">
-        <f>D8-$D4</f>
-        <v>29493</v>
+        <v>1</v>
       </c>
       <c r="L8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" s="1">
         <v>0</v>
       </c>
       <c r="N8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O8" s="1">
         <v>0</v>
       </c>
       <c r="P8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="1">
         <v>0</v>
       </c>
       <c r="R8" s="1">
-        <v>0</v>
+        <v>12728</v>
       </c>
       <c r="S8" s="1">
-        <v>0</v>
-      </c>
-      <c r="T8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20">
+        <v>502</v>
+      </c>
+      <c r="V8" s="1">
+        <v>3</v>
+      </c>
+      <c r="W8" s="1">
+        <v>4</v>
+      </c>
+      <c r="X8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
       <c r="A9" s="1">
         <v>4</v>
       </c>
@@ -5353,22 +5411,22 @@
         <v>401753</v>
       </c>
       <c r="C9" s="1">
-        <v>8</v>
+        <v>51809</v>
       </c>
       <c r="D9" s="1">
-        <v>51809</v>
+        <v>1740</v>
       </c>
       <c r="E9" s="1">
-        <v>8700</v>
+        <v>580</v>
       </c>
       <c r="F9" s="1">
-        <v>2900</v>
+        <v>3</v>
       </c>
       <c r="G9" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" s="1">
         <v>0</v>
@@ -5377,38 +5435,43 @@
         <v>0</v>
       </c>
       <c r="K9" s="1">
-        <f>D9-$D4</f>
-        <v>29606</v>
+        <v>1</v>
       </c>
       <c r="L9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9" s="1">
         <v>0</v>
       </c>
       <c r="N9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9" s="1">
         <v>0</v>
       </c>
       <c r="P9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q9" s="1">
         <v>0</v>
       </c>
       <c r="R9" s="1">
-        <v>0</v>
+        <v>12728</v>
       </c>
       <c r="S9" s="1">
-        <v>0</v>
-      </c>
-      <c r="T9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20">
+        <v>502</v>
+      </c>
+      <c r="V9" s="1">
+        <v>3</v>
+      </c>
+      <c r="W9" s="1">
+        <v>4</v>
+      </c>
+      <c r="X9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
       <c r="A10" s="1">
         <v>4</v>
       </c>
@@ -5416,19 +5479,19 @@
         <v>401753</v>
       </c>
       <c r="C10" s="1">
-        <v>9</v>
+        <v>54155</v>
       </c>
       <c r="D10" s="1">
-        <v>54155</v>
+        <v>1740</v>
       </c>
       <c r="E10" s="1">
-        <v>8700</v>
+        <v>0</v>
       </c>
       <c r="F10" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G10" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H10" s="1">
         <v>0</v>
@@ -5440,63 +5503,72 @@
         <v>0</v>
       </c>
       <c r="K10" s="1">
-        <f>D10-$D4</f>
-        <v>31952</v>
+        <v>1</v>
       </c>
       <c r="L10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10" s="1">
         <v>0</v>
       </c>
       <c r="N10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10" s="1">
         <v>0</v>
       </c>
       <c r="P10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q10" s="1">
         <v>0</v>
       </c>
       <c r="R10" s="1">
-        <v>0</v>
+        <v>12728</v>
       </c>
       <c r="S10" s="1">
-        <v>0</v>
-      </c>
-      <c r="T10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20">
+        <v>502</v>
+      </c>
+      <c r="V10" s="1">
+        <v>3</v>
+      </c>
+      <c r="W10" s="1">
+        <v>4</v>
+      </c>
+      <c r="X10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:24">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:24">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:24">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:24">
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:24">
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:14">
       <c r="I17" s="1"/>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="N18" s="1"/>
+    </row>
+    <row r="19" spans="1:14">
       <c r="F19" s="1" t="s">
         <v>59</v>
       </c>
@@ -5506,11 +5578,9 @@
       <c r="H19" s="1">
         <v>0</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="N19" s="1"/>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="1" t="s">
         <v>1</v>
       </c>
@@ -5529,318 +5599,359 @@
       <c r="H20" s="1">
         <v>2900</v>
       </c>
-      <c r="J20" s="1">
+      <c r="N20" s="1"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="1">
+        <v>1</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G21" s="1">
+        <v>6</v>
+      </c>
+      <c r="H21" s="1">
+        <v>2900</v>
+      </c>
+      <c r="N21" s="1"/>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="1">
+        <v>2</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="1">
+        <v>3200</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22" s="1">
+        <v>6</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
+      <c r="N22" s="1"/>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="1">
+        <v>3</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1600</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G23" s="1">
+        <v>6</v>
+      </c>
+      <c r="H23" s="1">
+        <v>2900</v>
+      </c>
+      <c r="N23" s="1"/>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="1">
+        <v>4</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2900</v>
+      </c>
+      <c r="N24" s="1"/>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="1">
+        <v>5</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2100</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" s="1">
+        <v>15</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="N25" s="1"/>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="1">
+        <v>6</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2900</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G26" s="1">
+        <v>4</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="1">
+        <v>7</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G27" s="1">
+        <v>4</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0</v>
+      </c>
+      <c r="J27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="1">
+        <v>8</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1600</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G28" s="1">
+        <v>6</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="1">
+        <v>9</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="1">
+        <v>900</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G29" s="1">
+        <v>6</v>
+      </c>
+      <c r="H29" s="1">
+        <v>2900</v>
+      </c>
+      <c r="J29" s="1">
+        <f>C5-$C4</f>
+        <v>7008</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="1">
+        <v>10</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="1">
+        <v>500</v>
+      </c>
+      <c r="J30" s="1">
+        <f>C6-$C4</f>
+        <v>27962</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="1">
+        <v>11</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0</v>
+      </c>
+      <c r="J31" s="1">
+        <f>C7-$C4</f>
+        <v>28562</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="1">
+        <v>12</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="1">
+        <v>500</v>
+      </c>
+      <c r="J32" s="1">
+        <f>C8-$C4</f>
+        <v>29493</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="1">
+        <v>13</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="1">
+        <v>800</v>
+      </c>
+      <c r="J33" s="1">
+        <f>C9-$C4</f>
+        <v>29606</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="1">
+        <v>14</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" s="1">
+        <v>200</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J34" s="1">
+        <f>C10-$C4</f>
+        <v>31952</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="1">
+        <v>15</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="1">
+        <v>5000</v>
+      </c>
+      <c r="F35" s="1">
         <f>SUM(H19:H23)</f>
         <v>8700</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="1">
-        <v>1</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" s="1">
-        <v>0</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G21" s="1">
-        <v>6</v>
-      </c>
-      <c r="H21" s="1">
-        <v>2900</v>
-      </c>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="1">
-        <v>2</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C22" s="1">
-        <v>3200</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G22" s="1">
-        <v>6</v>
-      </c>
-      <c r="H22" s="1">
-        <v>0</v>
-      </c>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="1">
-        <v>3</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="1">
+    <row r="36" spans="1:10">
+      <c r="A36" s="1">
+        <v>16</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="1">
+        <v>2400</v>
+      </c>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="1">
+        <v>17</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="1">
+        <v>18</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" s="1">
         <v>1600</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G23" s="1">
-        <v>6</v>
-      </c>
-      <c r="H23" s="1">
-        <v>2900</v>
-      </c>
-      <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="1">
-        <v>4</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C24" s="1">
-        <v>2900</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="1">
-        <v>5</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" s="1">
-        <v>2100</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G25" s="1">
-        <v>15</v>
-      </c>
-      <c r="H25" s="1">
-        <v>0</v>
-      </c>
-      <c r="J25" s="1">
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="1">
+        <v>19</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" s="1">
+        <v>1100</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="1">
+        <v>20</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="1">
+        <v>0</v>
+      </c>
+      <c r="F40" s="1">
         <f>SUM(H25:H29)</f>
         <v>2900</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="1">
-        <v>6</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C26" s="1">
-        <v>2900</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G26" s="1">
-        <v>4</v>
-      </c>
-      <c r="H26" s="1">
-        <v>0</v>
-      </c>
-      <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="1">
-        <v>7</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C27" s="1">
-        <v>0</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G27" s="1">
-        <v>4</v>
-      </c>
-      <c r="H27" s="1">
-        <v>0</v>
-      </c>
-      <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="1">
-        <v>8</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C28" s="1">
-        <v>1600</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G28" s="1">
-        <v>6</v>
-      </c>
-      <c r="H28" s="1">
-        <v>0</v>
-      </c>
-      <c r="J28" s="1"/>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="1">
-        <v>9</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="1">
-        <v>900</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G29" s="1">
-        <v>6</v>
-      </c>
-      <c r="H29" s="1">
-        <v>2900</v>
-      </c>
-      <c r="J29" s="1"/>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="1">
-        <v>10</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C30" s="1">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="1">
-        <v>11</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="1">
-        <v>12</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C32" s="1">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="1">
-        <v>13</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C33" s="1">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="1">
-        <v>14</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C34" s="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="1">
-        <v>15</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" s="1">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="1">
-        <v>16</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C36" s="1">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="1">
-        <v>17</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C37" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="1">
-        <v>18</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C38" s="1">
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="1">
-        <v>19</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C39" s="1">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="1">
-        <v>20</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C40" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:10">
       <c r="A41" s="1">
         <v>21</v>
       </c>
@@ -5849,6 +5960,967 @@
       </c>
       <c r="C41" s="1">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77970647-4F62-4C40-A931-952AB45C1877}">
+  <dimension ref="A1:S22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" customWidth="1"/>
+    <col min="4" max="5" width="7" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" customWidth="1"/>
+    <col min="7" max="7" width="4.140625" customWidth="1"/>
+    <col min="8" max="8" width="3.7109375" customWidth="1"/>
+    <col min="9" max="9" width="3.85546875" customWidth="1"/>
+    <col min="10" max="10" width="3.5703125" customWidth="1"/>
+    <col min="11" max="11" width="3.7109375" customWidth="1"/>
+    <col min="12" max="12" width="7.140625" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" customWidth="1"/>
+    <col min="14" max="14" width="5.28515625" customWidth="1"/>
+    <col min="15" max="16" width="3.28515625" customWidth="1"/>
+    <col min="17" max="17" width="3.140625" customWidth="1"/>
+    <col min="18" max="18" width="6.5703125" customWidth="1"/>
+    <col min="19" max="19" width="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="1">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1">
+        <v>401753</v>
+      </c>
+      <c r="C1" s="1">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2900</v>
+      </c>
+      <c r="E1" s="1">
+        <v>3320</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1">
+        <v>0</v>
+      </c>
+      <c r="J1" s="1">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1">
+        <v>0</v>
+      </c>
+      <c r="L1" s="1">
+        <v>0</v>
+      </c>
+      <c r="M1" s="1">
+        <v>0</v>
+      </c>
+      <c r="N1" s="1">
+        <v>1</v>
+      </c>
+      <c r="O1" s="1">
+        <v>0</v>
+      </c>
+      <c r="P1" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>0</v>
+      </c>
+      <c r="R1" s="1">
+        <v>12728</v>
+      </c>
+      <c r="S1" s="1">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="1">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>401753</v>
+      </c>
+      <c r="C2" s="1">
+        <v>7970</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2900</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2740</v>
+      </c>
+      <c r="F2" s="1">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
+        <v>1</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1">
+        <v>12728</v>
+      </c>
+      <c r="S2" s="1">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="1">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>401753</v>
+      </c>
+      <c r="C3" s="1">
+        <v>22203</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2900</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2740</v>
+      </c>
+      <c r="F3" s="1">
+        <v>5</v>
+      </c>
+      <c r="G3" s="1">
+        <v>4</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0</v>
+      </c>
+      <c r="R3" s="1">
+        <v>12728</v>
+      </c>
+      <c r="S3" s="1">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="1">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>401753</v>
+      </c>
+      <c r="C4" s="1">
+        <v>29211</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2320</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2740</v>
+      </c>
+      <c r="F4" s="1">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1">
+        <v>4</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <v>1</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>0</v>
+      </c>
+      <c r="R4" s="1">
+        <v>12728</v>
+      </c>
+      <c r="S4" s="1">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>401753</v>
+      </c>
+      <c r="C5" s="1">
+        <v>50165</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2320</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2160</v>
+      </c>
+      <c r="F5" s="1">
+        <v>4</v>
+      </c>
+      <c r="G5" s="1">
+        <v>3</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>1</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <v>12728</v>
+      </c>
+      <c r="S5" s="1">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>401753</v>
+      </c>
+      <c r="C6" s="1">
+        <v>50765</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1740</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2160</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3</v>
+      </c>
+      <c r="G6" s="1">
+        <v>3</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>1</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0</v>
+      </c>
+      <c r="N6" s="1">
+        <v>1</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+      <c r="P6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>0</v>
+      </c>
+      <c r="R6" s="1">
+        <v>12728</v>
+      </c>
+      <c r="S6" s="1">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="1">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1">
+        <v>401753</v>
+      </c>
+      <c r="C7" s="1">
+        <v>51696</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1740</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1160</v>
+      </c>
+      <c r="F7" s="1">
+        <v>3</v>
+      </c>
+      <c r="G7" s="1">
+        <v>2</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
+        <v>1</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>0</v>
+      </c>
+      <c r="R7" s="1">
+        <v>12728</v>
+      </c>
+      <c r="S7" s="1">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" s="1">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1">
+        <v>401753</v>
+      </c>
+      <c r="C8" s="1">
+        <v>51809</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1740</v>
+      </c>
+      <c r="E8" s="1">
+        <v>580</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0</v>
+      </c>
+      <c r="N8" s="1">
+        <v>1</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0</v>
+      </c>
+      <c r="P8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>0</v>
+      </c>
+      <c r="R8" s="1">
+        <v>12728</v>
+      </c>
+      <c r="S8" s="1">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" s="1">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1">
+        <v>401753</v>
+      </c>
+      <c r="C9" s="1">
+        <v>54155</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1740</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>1</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
+        <v>1</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0</v>
+      </c>
+      <c r="R9" s="1">
+        <v>12728</v>
+      </c>
+      <c r="S9" s="1">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="B14" s="1">
+        <v>401753</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2900</v>
+      </c>
+      <c r="E14" s="1">
+        <v>3320</v>
+      </c>
+      <c r="F14" s="1">
+        <v>5</v>
+      </c>
+      <c r="G14" s="1">
+        <v>5</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M14" s="1">
+        <v>12728</v>
+      </c>
+      <c r="N14" s="1">
+        <v>502</v>
+      </c>
+      <c r="O14" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="B15" s="1">
+        <v>401753</v>
+      </c>
+      <c r="C15" s="1">
+        <v>7970</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2900</v>
+      </c>
+      <c r="E15" s="1">
+        <v>2740</v>
+      </c>
+      <c r="F15" s="1">
+        <v>5</v>
+      </c>
+      <c r="G15" s="1">
+        <v>4</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M15" s="1">
+        <v>12728</v>
+      </c>
+      <c r="N15" s="1">
+        <v>502</v>
+      </c>
+      <c r="O15" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="B16" s="1">
+        <v>401753</v>
+      </c>
+      <c r="C16" s="1">
+        <v>22203</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2900</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2740</v>
+      </c>
+      <c r="F16" s="1">
+        <v>5</v>
+      </c>
+      <c r="G16" s="1">
+        <v>4</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M16" s="1">
+        <v>12728</v>
+      </c>
+      <c r="N16" s="1">
+        <v>502</v>
+      </c>
+      <c r="O16" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15">
+      <c r="B17" s="1">
+        <v>401753</v>
+      </c>
+      <c r="C17" s="1">
+        <v>29211</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2320</v>
+      </c>
+      <c r="E17" s="1">
+        <v>2740</v>
+      </c>
+      <c r="F17" s="1">
+        <v>4</v>
+      </c>
+      <c r="G17" s="1">
+        <v>4</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M17" s="1">
+        <v>12728</v>
+      </c>
+      <c r="N17" s="1">
+        <v>502</v>
+      </c>
+      <c r="O17" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15">
+      <c r="B18" s="1">
+        <v>401753</v>
+      </c>
+      <c r="C18" s="1">
+        <v>50165</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2320</v>
+      </c>
+      <c r="E18" s="1">
+        <v>2160</v>
+      </c>
+      <c r="F18" s="1">
+        <v>4</v>
+      </c>
+      <c r="G18" s="1">
+        <v>3</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M18" s="1">
+        <v>12728</v>
+      </c>
+      <c r="N18" s="1">
+        <v>502</v>
+      </c>
+      <c r="O18" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15">
+      <c r="B19" s="1">
+        <v>401753</v>
+      </c>
+      <c r="C19" s="1">
+        <v>50765</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1740</v>
+      </c>
+      <c r="E19" s="1">
+        <v>2160</v>
+      </c>
+      <c r="F19" s="1">
+        <v>3</v>
+      </c>
+      <c r="G19" s="1">
+        <v>3</v>
+      </c>
+      <c r="H19" s="1">
+        <v>1</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M19" s="1">
+        <v>12728</v>
+      </c>
+      <c r="N19" s="1">
+        <v>502</v>
+      </c>
+      <c r="O19" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15">
+      <c r="B20" s="1">
+        <v>401753</v>
+      </c>
+      <c r="C20" s="1">
+        <v>51696</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1740</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1160</v>
+      </c>
+      <c r="F20" s="1">
+        <v>3</v>
+      </c>
+      <c r="G20" s="1">
+        <v>2</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M20" s="1">
+        <v>12728</v>
+      </c>
+      <c r="N20" s="1">
+        <v>502</v>
+      </c>
+      <c r="O20" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15">
+      <c r="B21" s="1">
+        <v>401753</v>
+      </c>
+      <c r="C21" s="1">
+        <v>51809</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1740</v>
+      </c>
+      <c r="E21" s="1">
+        <v>580</v>
+      </c>
+      <c r="F21" s="1">
+        <v>3</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M21" s="1">
+        <v>12728</v>
+      </c>
+      <c r="N21" s="1">
+        <v>502</v>
+      </c>
+      <c r="O21" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15">
+      <c r="B22" s="1">
+        <v>401753</v>
+      </c>
+      <c r="C22" s="1">
+        <v>54155</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1740</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <v>3</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M22" s="1">
+        <v>12728</v>
+      </c>
+      <c r="N22" s="1">
+        <v>502</v>
+      </c>
+      <c r="O22" s="1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished single map dataframe export
</commit_message>
<xml_diff>
--- a/webscrapping/matches/model/Book1.xlsx
+++ b/webscrapping/matches/model/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Meus Documentos\Python\Notebooks\Datascience\Classification_datascience\webscrapping\matches\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26DC98F3-11BA-46D0-8505-2DCE4B536D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F39CAC-B8F1-4289-8F11-C51A2C561EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{1C43445C-3BFE-43FA-8FCA-AB69F1532CAF}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="24450" windowHeight="14670" activeTab="5" xr2:uid="{1C43445C-3BFE-43FA-8FCA-AB69F1532CAF}"/>
   </bookViews>
   <sheets>
     <sheet name="overview" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="events" sheetId="4" r:id="rId4"/>
     <sheet name="final_sheet" sheetId="5" r:id="rId5"/>
     <sheet name="test" sheetId="6" r:id="rId6"/>
+    <sheet name="scrap" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="128">
   <si>
     <t>number</t>
   </si>
@@ -677,6 +678,57 @@
   </si>
   <si>
     <t>'Icebox'</t>
+  </si>
+  <si>
+    <t>stamp</t>
+  </si>
+  <si>
+    <t>defgun</t>
+  </si>
+  <si>
+    <t>atkgun</t>
+  </si>
+  <si>
+    <t>atkali</t>
+  </si>
+  <si>
+    <t>defali</t>
+  </si>
+  <si>
+    <t>op</t>
+  </si>
+  <si>
+    <t>odin</t>
+  </si>
+  <si>
+    <t>2bp</t>
+  </si>
+  <si>
+    <t>1bp</t>
+  </si>
+  <si>
+    <t>map</t>
+  </si>
+  <si>
+    <t>match</t>
+  </si>
+  <si>
+    <t>series</t>
+  </si>
+  <si>
+    <t>bo</t>
+  </si>
+  <si>
+    <t>winner</t>
+  </si>
+  <si>
+    <t>https://runitback.gg/series/12728?match=25608&amp;round=1&amp;tab=replay</t>
+  </si>
+  <si>
+    <t>https://runitback.gg/series/12728</t>
+  </si>
+  <si>
+    <t>https://runitback.gg/series/12728?match=25609&amp;round=1&amp;tab=round-stats</t>
   </si>
 </sst>
 </file>
@@ -3843,7 +3895,7 @@
   <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4838,8 +4890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F1A27BA-379F-49F7-9EA2-31A14ABA745C}">
   <dimension ref="A1:X41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S1" sqref="A1:S10"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5969,10 +6021,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77970647-4F62-4C40-A931-952AB45C1877}">
-  <dimension ref="A1:S22"/>
+  <dimension ref="A1:AH37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5981,16 +6033,17 @@
     <col min="2" max="2" width="8" customWidth="1"/>
     <col min="3" max="3" width="6.85546875" customWidth="1"/>
     <col min="4" max="5" width="7" customWidth="1"/>
-    <col min="6" max="6" width="5.140625" customWidth="1"/>
-    <col min="7" max="7" width="4.140625" customWidth="1"/>
-    <col min="8" max="8" width="3.7109375" customWidth="1"/>
-    <col min="9" max="9" width="3.85546875" customWidth="1"/>
-    <col min="10" max="10" width="3.5703125" customWidth="1"/>
-    <col min="11" max="11" width="3.7109375" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" customWidth="1"/>
+    <col min="8" max="8" width="5" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+    <col min="11" max="11" width="4.140625" customWidth="1"/>
     <col min="12" max="12" width="7.140625" customWidth="1"/>
     <col min="13" max="13" width="7.7109375" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" customWidth="1"/>
-    <col min="15" max="16" width="3.28515625" customWidth="1"/>
+    <col min="14" max="14" width="5.5703125" customWidth="1"/>
+    <col min="15" max="15" width="3.42578125" customWidth="1"/>
+    <col min="16" max="16" width="7.140625" customWidth="1"/>
     <col min="17" max="17" width="3.140625" customWidth="1"/>
     <col min="18" max="18" width="6.5703125" customWidth="1"/>
     <col min="19" max="19" width="5" customWidth="1"/>
@@ -6527,9 +6580,59 @@
         <v>502</v>
       </c>
     </row>
+    <row r="13" spans="1:19">
+      <c r="B13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+    </row>
     <row r="14" spans="1:19">
       <c r="B14" s="1">
-        <v>401753</v>
+        <v>401758</v>
       </c>
       <c r="C14" s="1">
         <v>0</v>
@@ -6538,7 +6641,7 @@
         <v>2900</v>
       </c>
       <c r="E14" s="1">
-        <v>3320</v>
+        <v>2120</v>
       </c>
       <c r="F14" s="1">
         <v>5</v>
@@ -6547,7 +6650,7 @@
         <v>5</v>
       </c>
       <c r="H14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" s="1">
         <v>0</v>
@@ -6570,28 +6673,31 @@
       <c r="O14" s="1">
         <v>3</v>
       </c>
+      <c r="P14" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:19">
       <c r="B15" s="1">
-        <v>401753</v>
+        <v>401758</v>
       </c>
       <c r="C15" s="1">
-        <v>7970</v>
+        <v>50476</v>
       </c>
       <c r="D15" s="1">
-        <v>2900</v>
+        <v>2320</v>
       </c>
       <c r="E15" s="1">
-        <v>2740</v>
+        <v>2120</v>
       </c>
       <c r="F15" s="1">
+        <v>4</v>
+      </c>
+      <c r="G15" s="1">
         <v>5</v>
       </c>
-      <c r="G15" s="1">
-        <v>4</v>
-      </c>
       <c r="H15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" s="1">
         <v>0</v>
@@ -6614,28 +6720,31 @@
       <c r="O15" s="1">
         <v>3</v>
       </c>
+      <c r="P15" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:19">
       <c r="B16" s="1">
-        <v>401753</v>
+        <v>401758</v>
       </c>
       <c r="C16" s="1">
-        <v>22203</v>
+        <v>53699</v>
       </c>
       <c r="D16" s="1">
-        <v>2900</v>
+        <v>2320</v>
       </c>
       <c r="E16" s="1">
-        <v>2740</v>
+        <v>2120</v>
       </c>
       <c r="F16" s="1">
+        <v>4</v>
+      </c>
+      <c r="G16" s="1">
         <v>5</v>
       </c>
-      <c r="G16" s="1">
-        <v>4</v>
-      </c>
       <c r="H16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" s="1">
         <v>0</v>
@@ -6658,28 +6767,31 @@
       <c r="O16" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="2:15">
+      <c r="P16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:34">
       <c r="B17" s="1">
-        <v>401753</v>
+        <v>401758</v>
       </c>
       <c r="C17" s="1">
-        <v>29211</v>
+        <v>53987</v>
       </c>
       <c r="D17" s="1">
-        <v>2320</v>
+        <v>1740</v>
       </c>
       <c r="E17" s="1">
-        <v>2740</v>
+        <v>2120</v>
       </c>
       <c r="F17" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G17" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" s="1">
         <v>0</v>
@@ -6702,28 +6814,31 @@
       <c r="O17" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="2:15">
+      <c r="P17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:34">
       <c r="B18" s="1">
-        <v>401753</v>
+        <v>401758</v>
       </c>
       <c r="C18" s="1">
-        <v>50165</v>
+        <v>54090</v>
       </c>
       <c r="D18" s="1">
-        <v>2320</v>
+        <v>1740</v>
       </c>
       <c r="E18" s="1">
-        <v>2160</v>
+        <v>1540</v>
       </c>
       <c r="F18" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G18" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" s="1">
         <v>0</v>
@@ -6746,28 +6861,31 @@
       <c r="O18" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="2:15">
+      <c r="P18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:34">
       <c r="B19" s="1">
-        <v>401753</v>
+        <v>401758</v>
       </c>
       <c r="C19" s="1">
-        <v>50765</v>
+        <v>55706</v>
       </c>
       <c r="D19" s="1">
-        <v>1740</v>
+        <v>1160</v>
       </c>
       <c r="E19" s="1">
-        <v>2160</v>
+        <v>1540</v>
       </c>
       <c r="F19" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G19" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19" s="1">
         <v>0</v>
@@ -6790,25 +6908,28 @@
       <c r="O19" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="2:15">
+      <c r="P19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:34">
       <c r="B20" s="1">
-        <v>401753</v>
+        <v>401758</v>
       </c>
       <c r="C20" s="1">
-        <v>51696</v>
+        <v>77867</v>
       </c>
       <c r="D20" s="1">
-        <v>1740</v>
+        <v>580</v>
       </c>
       <c r="E20" s="1">
-        <v>1160</v>
+        <v>1540</v>
       </c>
       <c r="F20" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G20" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H20" s="1">
         <v>0</v>
@@ -6834,25 +6955,28 @@
       <c r="O20" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="2:15">
+      <c r="P20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:34">
       <c r="B21" s="1">
-        <v>401753</v>
+        <v>401758</v>
       </c>
       <c r="C21" s="1">
-        <v>51809</v>
+        <v>79124</v>
       </c>
       <c r="D21" s="1">
-        <v>1740</v>
+        <v>580</v>
       </c>
       <c r="E21" s="1">
-        <v>580</v>
+        <v>1320</v>
       </c>
       <c r="F21" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G21" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H21" s="1">
         <v>0</v>
@@ -6878,25 +7002,28 @@
       <c r="O21" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="2:15">
+      <c r="P21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:34">
       <c r="B22" s="1">
-        <v>401753</v>
+        <v>401758</v>
       </c>
       <c r="C22" s="1">
-        <v>54155</v>
+        <v>81219</v>
       </c>
       <c r="D22" s="1">
-        <v>1740</v>
+        <v>580</v>
       </c>
       <c r="E22" s="1">
-        <v>0</v>
+        <v>1160</v>
       </c>
       <c r="F22" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G22" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H22" s="1">
         <v>0</v>
@@ -6921,6 +7048,210 @@
       </c>
       <c r="O22" s="1">
         <v>3</v>
+      </c>
+      <c r="P22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:34">
+      <c r="B23" s="1">
+        <v>401758</v>
+      </c>
+      <c r="C23" s="1">
+        <v>84771</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1160</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1">
+        <v>2</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M23" s="1">
+        <v>12728</v>
+      </c>
+      <c r="N23" s="1">
+        <v>502</v>
+      </c>
+      <c r="O23" s="1">
+        <v>3</v>
+      </c>
+      <c r="P23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:34">
+      <c r="B24" s="1">
+        <v>401758</v>
+      </c>
+      <c r="C24" s="1">
+        <v>85901</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1160</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1">
+        <v>2</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0</v>
+      </c>
+      <c r="K24" s="1">
+        <v>0</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M24" s="1">
+        <v>12728</v>
+      </c>
+      <c r="N24" s="1">
+        <v>502</v>
+      </c>
+      <c r="O24" s="1">
+        <v>3</v>
+      </c>
+      <c r="P24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:34">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+    </row>
+    <row r="26" spans="2:34">
+      <c r="AH26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:34">
+      <c r="AH27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:34">
+      <c r="AH28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:34">
+      <c r="AH29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:34">
+      <c r="AH30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:34">
+      <c r="AH31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:34">
+      <c r="AH32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="34:34">
+      <c r="AH33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="34:34">
+      <c r="AH34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="34:34">
+      <c r="AH35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="34:34">
+      <c r="AH36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="34:34">
+      <c r="AH37">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3B0D7F3-1E82-4CDC-91F7-DC7DE9308424}">
+  <dimension ref="B3:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3" spans="2:2">
+      <c r="B3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>